<commit_message>
add new dq checks
</commit_message>
<xml_diff>
--- a/HW3_approach/TestCas_myVersion.xlsx
+++ b/HW3_approach/TestCas_myVersion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitalii_Stetsenko\Desktop\intermediate_course\Data Testing Approaches - HomeTask by Volha Melnikava_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitalii_Stetsenko\PycharmProjects\Course_Intermediate_DQE\HW3_approach\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D3B7BD-2A9E-458B-8B2B-640B407E57D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B61B1AA-1971-4778-81B9-066D42B59835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DQ Checks'!$B$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="164">
   <si>
     <t>Source</t>
   </si>
@@ -68,15 +68,6 @@
     <t>Forecast</t>
   </si>
   <si>
-    <t>Completeness by …</t>
-  </si>
-  <si>
-    <t>Excel file name that should be used to cover this case</t>
-  </si>
-  <si>
-    <t>s3://test-bucket/raw/forecast/run_dt=20200213T150401</t>
-  </si>
-  <si>
     <t>No.</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -95,12 +86,6 @@
     <t>Hive Query</t>
   </si>
   <si>
-    <t>LZ, RAW, CLEANSED</t>
-  </si>
-  <si>
-    <t>All or some specific columns</t>
-  </si>
-  <si>
     <t>Check Type</t>
   </si>
   <si>
@@ -113,9 +98,6 @@
     <t>LZ</t>
   </si>
   <si>
-    <t>Consistency by records</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
@@ -299,15 +281,6 @@
     <t>Column value</t>
   </si>
   <si>
-    <t>Check incremental load</t>
-  </si>
-  <si>
-    <t>Verify that new data inserted and updated for already loaded records</t>
-  </si>
-  <si>
-    <t>New data inserted and updated for already loaded records</t>
-  </si>
-  <si>
     <t>Forecast_20230301.pdf    Forecast_20230301.xlsx</t>
   </si>
   <si>
@@ -486,6 +459,84 @@
   </si>
   <si>
     <t>Check that values in  InsertDateTime, UpdateDateTime columns specified in UTC time zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New data inserted </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that new data inserted </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forecast_20230309.xlsx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check incremental new data load </t>
+  </si>
+  <si>
+    <t>Verify that valid data don’t put in quarantine</t>
+  </si>
+  <si>
+    <t>Check incremental updated data loaded</t>
+  </si>
+  <si>
+    <t>Verify that updated data uploaded without changing old data</t>
+  </si>
+  <si>
+    <t>The data from both files 'Forecast_20230308.xlsx' and  'Forecast_20230308.xlsx' persist in incremental</t>
+  </si>
+  <si>
+    <t>No data added to quarantine</t>
+  </si>
+  <si>
+    <t>s3://test-bucket/cleansed/forecast/run_dt=20230301</t>
+  </si>
+  <si>
+    <t>SELECT * FROM forecast_cleansed WHERE run_dt = CURRENT_DATETIME</t>
+  </si>
+  <si>
+    <t>Uniquness by primary key</t>
+  </si>
+  <si>
+    <t>Accuracy by system columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> InsertDateTime, UpdateDateTime, file_name</t>
+  </si>
+  <si>
+    <t>SELECT * FROM forecast_cleansed WHERE UpdateDateTime IS NOT NULL and file_name = 'Forecast_20230309.xlsx'</t>
+  </si>
+  <si>
+    <t>InsertDateTime column not updated. UpdateDateTime and file_name were updated. Query shows 7 records</t>
+  </si>
+  <si>
+    <t>RAW partitioning</t>
+  </si>
+  <si>
+    <t>CLEANSED partitioning</t>
+  </si>
+  <si>
+    <t>Check partitioning in CLEANSED</t>
+  </si>
+  <si>
+    <t>Check partitioning in RAW</t>
+  </si>
+  <si>
+    <t>Timeless by apearing new data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forecast_20230301.xlsx </t>
+  </si>
+  <si>
+    <t>Timeless by old file</t>
+  </si>
+  <si>
+    <t>Pipeline doesn't process already processed files</t>
+  </si>
+  <si>
+    <t>Pipeline process only data that got before 5 PM UTC of current day. Pipeline doesn't break or process new file if it got it during work of pipeline.</t>
+  </si>
+  <si>
+    <t>Completeness by records</t>
   </si>
 </sst>
 </file>
@@ -617,7 +668,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -648,6 +699,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -930,9 +984,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCCC296-2BB6-4C22-A4E3-D35AA4A9CD78}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -951,19 +1005,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>6</v>
@@ -972,15 +1026,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -989,19 +1043,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1012,19 +1066,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="H4" s="7"/>
     </row>
@@ -1034,19 +1088,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H5" s="7"/>
     </row>
@@ -1056,19 +1110,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>154</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>54</v>
+        <v>157</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -1078,328 +1132,394 @@
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" t="s">
-        <v>69</v>
+        <v>155</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>56</v>
+        <v>156</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>57</v>
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>59</v>
+        <v>65</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>142</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>79</v>
+        <v>146</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>78</v>
+        <v>103</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="2:8" ht="58.2" x14ac:dyDescent="0.35">
+      <c r="B17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="2:8" ht="45" x14ac:dyDescent="0.35">
+      <c r="B18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
         <v>60</v>
       </c>
-      <c r="D13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.35">
-      <c r="B14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.35">
-      <c r="B15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="E20" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="F24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="G22" s="7"/>
+    </row>
+    <row r="25" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>136</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1409,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,7 +1550,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1451,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>6</v>
@@ -1468,29 +1588,33 @@
         <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+        <v>107</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>7</v>
@@ -1498,21 +1622,23 @@
       <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>22</v>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" s="7"/>
+        <v>85</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="I3" s="7" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -1520,31 +1646,31 @@
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -1552,31 +1678,29 @@
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>160</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>33</v>
+        <v>159</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -1584,31 +1708,29 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>124</v>
+        <v>159</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1616,31 +1738,29 @@
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>129</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="H7" s="7"/>
       <c r="I7" s="7" t="s">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1648,31 +1768,31 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:14" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>163</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1680,31 +1800,31 @@
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:14" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>126</v>
+        <v>23</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -1712,31 +1832,31 @@
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>118</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>101</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -1744,31 +1864,31 @@
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -1776,31 +1896,31 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -1808,31 +1928,31 @@
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -1840,31 +1960,31 @@
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -1872,30 +1992,31 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="I15" t="s">
-        <v>136</v>
       </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -1903,30 +2024,31 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="I16" t="s">
-        <v>136</v>
+        <v>41</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
@@ -1934,30 +2056,30 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>138</v>
+        <v>89</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="I17" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -1965,31 +2087,30 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="I18" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
@@ -1997,48 +2118,95 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+    <row r="19" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19" t="s">
+        <v>127</v>
+      </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I20" t="s">
+        <v>127</v>
+      </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="B21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>153</v>
+      </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -2109,8 +2277,44 @@
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
     </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:I1" xr:uid="{DB9E0EBC-55C6-446F-BB54-B15842229FFE}"/>
+  <autoFilter ref="B1:I1" xr:uid="{DB9E0EBC-55C6-446F-BB54-B15842229FFE}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I18">
+      <sortCondition descending="1" ref="C1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>